<commit_message>
acréscimo de comentários e testes
</commit_message>
<xml_diff>
--- a/RPA-checkpoint-3-acesso-queue/dados_ibge/dados_ibge_cidade.xlsx
+++ b/RPA-checkpoint-3-acesso-queue/dados_ibge/dados_ibge_cidade.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gust_\Documents\UiPath\RPA-checkpoint-3-acesso-queue\dados_ibge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gust_\Documents\GitHub\rpa-cp3-fiap\RPA-checkpoint-3-acesso-queue\dados_ibge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E621A33E-BD91-4177-94BC-417FF7CCE7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D6BCEC-CE01-4970-8E37-2CB188DB1EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28B6AF94-7C28-4272-8876-8D3588CAED95}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,17 +631,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7bc641a7-997f-4048-a412-d593c6319208">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100223DA578DE33E44E8DD11C312C11F0C0" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="346ab74657b96891a140619d15345a6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7bc641a7-997f-4048-a412-d593c6319208" xmlns:ns3="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01055a3472747d3415116a8d374e9951" ns2:_="" ns3:_="">
     <xsd:import namespace="7bc641a7-997f-4048-a412-d593c6319208"/>
@@ -870,7 +859,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -879,19 +868,18 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7bc641a7-997f-4048-a412-d593c6319208">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83A287C5-F434-4695-83F0-EED2E79F2819}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9"/>
-    <ds:schemaRef ds:uri="7bc641a7-997f-4048-a412-d593c6319208"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{342E861F-38C4-4FCE-AB34-3E1BC43BC858}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -910,10 +898,22 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D25C0718-6F6F-4264-BAB0-F03BD7013163}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83A287C5-F434-4695-83F0-EED2E79F2819}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9"/>
+    <ds:schemaRef ds:uri="7bc641a7-997f-4048-a412-d593c6319208"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Acréscimo de tratamento de exceções
</commit_message>
<xml_diff>
--- a/RPA-checkpoint-3-acesso-queue/dados_ibge/dados_ibge_cidade.xlsx
+++ b/RPA-checkpoint-3-acesso-queue/dados_ibge/dados_ibge_cidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gust_\Documents\GitHub\rpa-cp3-fiap\RPA-checkpoint-3-acesso-queue\dados_ibge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D6BCEC-CE01-4970-8E37-2CB188DB1EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A264FC56-8B65-4AFC-AB65-D12F7AF151D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{28B6AF94-7C28-4272-8876-8D3588CAED95}"/>
   </bookViews>
@@ -129,12 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174E5EC6-57C0-4B4A-9117-7632484C994F}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,9 +573,6 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K2" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -591,18 +587,18 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="A1:G18"/>
+      <selection activeCell="H19" sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
@@ -617,7 +613,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,6 +627,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7bc641a7-997f-4048-a412-d593c6319208">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100223DA578DE33E44E8DD11C312C11F0C0" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="346ab74657b96891a140619d15345a6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7bc641a7-997f-4048-a412-d593c6319208" xmlns:ns3="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01055a3472747d3415116a8d374e9951" ns2:_="" ns3:_="">
     <xsd:import namespace="7bc641a7-997f-4048-a412-d593c6319208"/>
@@ -859,7 +866,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -868,18 +875,19 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7bc641a7-997f-4048-a412-d593c6319208">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83A287C5-F434-4695-83F0-EED2E79F2819}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9"/>
+    <ds:schemaRef ds:uri="7bc641a7-997f-4048-a412-d593c6319208"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{342E861F-38C4-4FCE-AB34-3E1BC43BC858}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -898,22 +906,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D25C0718-6F6F-4264-BAB0-F03BD7013163}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83A287C5-F434-4695-83F0-EED2E79F2819}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9"/>
-    <ds:schemaRef ds:uri="7bc641a7-997f-4048-a412-d593c6319208"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>